<commit_message>
add v2 for quickLook_v2
</commit_message>
<xml_diff>
--- a/notebookscc/ana_summer2021/logbooks/auxtelholologbook_2021_07_07_v4.0.xlsx
+++ b/notebookscc/ana_summer2021/logbooks/auxtelholologbook_2021_07_07_v4.0.xlsx
@@ -1332,7 +1332,7 @@
         <v>600</v>
       </c>
       <c r="S2">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="V2" t="s">
         <v>276</v>
@@ -6206,10 +6206,10 @@
         <v>5.4</v>
       </c>
       <c r="R87">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="S87">
-        <v>2140</v>
+        <v>2200</v>
       </c>
       <c r="V87" t="s">
         <v>276</v>
@@ -6274,7 +6274,7 @@
         <v>400</v>
       </c>
       <c r="S88">
-        <v>2200</v>
+        <v>2300</v>
       </c>
       <c r="V88" t="s">
         <v>276</v>
@@ -6404,7 +6404,7 @@
         <v>400</v>
       </c>
       <c r="S90">
-        <v>2250</v>
+        <v>2400</v>
       </c>
       <c r="V90" t="s">
         <v>276</v>
@@ -6599,7 +6599,7 @@
         <v>300</v>
       </c>
       <c r="S93">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="V93" t="s">
         <v>276</v>
@@ -6661,10 +6661,10 @@
         <v>6.8</v>
       </c>
       <c r="R94">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="S94">
-        <v>2000</v>
+        <v>2100</v>
       </c>
       <c r="V94" t="s">
         <v>276</v>
@@ -6924,7 +6924,7 @@
         <v>300</v>
       </c>
       <c r="S98">
-        <v>2400</v>
+        <v>2500</v>
       </c>
       <c r="V98" t="s">
         <v>276</v>
@@ -6985,8 +6985,20 @@
       <c r="Q99">
         <v>6.3</v>
       </c>
+      <c r="R99">
+        <v>200</v>
+      </c>
+      <c r="S99">
+        <v>1800</v>
+      </c>
       <c r="V99" t="s">
         <v>276</v>
+      </c>
+      <c r="W99">
+        <v>1</v>
+      </c>
+      <c r="X99">
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:24">
@@ -7038,8 +7050,20 @@
       <c r="Q100">
         <v>6.3</v>
       </c>
+      <c r="R100">
+        <v>200</v>
+      </c>
+      <c r="S100">
+        <v>1800</v>
+      </c>
       <c r="V100" t="s">
         <v>276</v>
+      </c>
+      <c r="W100">
+        <v>1</v>
+      </c>
+      <c r="X100">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:24">
@@ -7091,8 +7115,20 @@
       <c r="Q101">
         <v>6.9</v>
       </c>
+      <c r="R101">
+        <v>200</v>
+      </c>
+      <c r="S101">
+        <v>2100</v>
+      </c>
       <c r="V101" t="s">
         <v>276</v>
+      </c>
+      <c r="W101">
+        <v>1</v>
+      </c>
+      <c r="X101">
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:24">
@@ -7144,8 +7180,20 @@
       <c r="Q102">
         <v>6.9</v>
       </c>
+      <c r="R102">
+        <v>200</v>
+      </c>
+      <c r="S102">
+        <v>2200</v>
+      </c>
       <c r="V102" t="s">
         <v>276</v>
+      </c>
+      <c r="W102">
+        <v>1</v>
+      </c>
+      <c r="X102">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:24">
@@ -7197,8 +7245,20 @@
       <c r="Q103">
         <v>7.1</v>
       </c>
+      <c r="R103">
+        <v>200</v>
+      </c>
+      <c r="S103">
+        <v>2200</v>
+      </c>
       <c r="V103" t="s">
         <v>276</v>
+      </c>
+      <c r="W103">
+        <v>1</v>
+      </c>
+      <c r="X103">
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:24">
@@ -7250,8 +7310,20 @@
       <c r="Q104">
         <v>8.4</v>
       </c>
+      <c r="R104">
+        <v>200</v>
+      </c>
+      <c r="S104">
+        <v>2200</v>
+      </c>
       <c r="V104" t="s">
         <v>276</v>
+      </c>
+      <c r="W104">
+        <v>1</v>
+      </c>
+      <c r="X104">
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:24">
@@ -7303,8 +7375,20 @@
       <c r="Q105">
         <v>8.4</v>
       </c>
+      <c r="R105">
+        <v>200</v>
+      </c>
+      <c r="S105">
+        <v>2500</v>
+      </c>
       <c r="V105" t="s">
         <v>276</v>
+      </c>
+      <c r="W105">
+        <v>1</v>
+      </c>
+      <c r="X105">
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:24">
@@ -7356,8 +7440,20 @@
       <c r="Q106">
         <v>6.6</v>
       </c>
+      <c r="R106">
+        <v>100</v>
+      </c>
+      <c r="S106">
+        <v>1800</v>
+      </c>
       <c r="V106" t="s">
         <v>276</v>
+      </c>
+      <c r="W106">
+        <v>1</v>
+      </c>
+      <c r="X106">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:24">
@@ -7409,8 +7505,20 @@
       <c r="Q107">
         <v>6.6</v>
       </c>
+      <c r="R107">
+        <v>100</v>
+      </c>
+      <c r="S107">
+        <v>1900</v>
+      </c>
       <c r="V107" t="s">
         <v>276</v>
+      </c>
+      <c r="W107">
+        <v>1</v>
+      </c>
+      <c r="X107">
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:24">
@@ -7462,8 +7570,20 @@
       <c r="Q108">
         <v>6.6</v>
       </c>
+      <c r="R108">
+        <v>100</v>
+      </c>
+      <c r="S108">
+        <v>2100</v>
+      </c>
       <c r="V108" t="s">
         <v>276</v>
+      </c>
+      <c r="W108">
+        <v>1</v>
+      </c>
+      <c r="X108">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:24">
@@ -7515,8 +7635,20 @@
       <c r="Q109">
         <v>6.6</v>
       </c>
+      <c r="R109">
+        <v>120</v>
+      </c>
+      <c r="S109">
+        <v>2100</v>
+      </c>
       <c r="V109" t="s">
         <v>276</v>
+      </c>
+      <c r="W109">
+        <v>1</v>
+      </c>
+      <c r="X109">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:24">
@@ -7568,8 +7700,20 @@
       <c r="Q110">
         <v>7.9</v>
       </c>
+      <c r="R110">
+        <v>200</v>
+      </c>
+      <c r="S110">
+        <v>2200</v>
+      </c>
       <c r="V110" t="s">
         <v>276</v>
+      </c>
+      <c r="W110">
+        <v>1</v>
+      </c>
+      <c r="X110">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:24">
@@ -7621,8 +7765,20 @@
       <c r="Q111">
         <v>7.9</v>
       </c>
+      <c r="R111">
+        <v>150</v>
+      </c>
+      <c r="S111">
+        <v>2300</v>
+      </c>
       <c r="V111" t="s">
         <v>276</v>
+      </c>
+      <c r="W111">
+        <v>1</v>
+      </c>
+      <c r="X111">
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:24">
@@ -7674,11 +7830,23 @@
       <c r="Q112">
         <v>8.1</v>
       </c>
+      <c r="R112">
+        <v>150</v>
+      </c>
+      <c r="S112">
+        <v>2400</v>
+      </c>
       <c r="V112" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="113" spans="1:22">
+      <c r="W112">
+        <v>1</v>
+      </c>
+      <c r="X112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -7727,11 +7895,23 @@
       <c r="Q113">
         <v>8.1</v>
       </c>
+      <c r="R113">
+        <v>50</v>
+      </c>
+      <c r="S113">
+        <v>2300</v>
+      </c>
       <c r="V113" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="114" spans="1:22">
+      <c r="W113">
+        <v>1</v>
+      </c>
+      <c r="X113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -7780,11 +7960,23 @@
       <c r="Q114">
         <v>7.6</v>
       </c>
+      <c r="R114">
+        <v>50</v>
+      </c>
+      <c r="S114">
+        <v>1800</v>
+      </c>
       <c r="V114" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="115" spans="1:22">
+      <c r="W114">
+        <v>1</v>
+      </c>
+      <c r="X114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -7833,11 +8025,23 @@
       <c r="Q115">
         <v>7.6</v>
       </c>
+      <c r="R115">
+        <v>50</v>
+      </c>
+      <c r="S115">
+        <v>1800</v>
+      </c>
       <c r="V115" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="116" spans="1:22">
+      <c r="W115">
+        <v>1</v>
+      </c>
+      <c r="X115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -7886,11 +8090,23 @@
       <c r="Q116">
         <v>6.8</v>
       </c>
+      <c r="R116">
+        <v>50</v>
+      </c>
+      <c r="S116">
+        <v>2100</v>
+      </c>
       <c r="V116" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="117" spans="1:22">
+      <c r="W116">
+        <v>1</v>
+      </c>
+      <c r="X116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -7939,11 +8155,23 @@
       <c r="Q117">
         <v>6.8</v>
       </c>
+      <c r="R117">
+        <v>50</v>
+      </c>
+      <c r="S117">
+        <v>2200</v>
+      </c>
       <c r="V117" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="118" spans="1:22">
+      <c r="W117">
+        <v>1</v>
+      </c>
+      <c r="X117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -7992,11 +8220,23 @@
       <c r="Q118">
         <v>7.1</v>
       </c>
+      <c r="R118">
+        <v>50</v>
+      </c>
+      <c r="S118">
+        <v>2300</v>
+      </c>
       <c r="V118" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="119" spans="1:22">
+      <c r="W118">
+        <v>1</v>
+      </c>
+      <c r="X118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -8045,11 +8285,23 @@
       <c r="Q119">
         <v>8.199999999999999</v>
       </c>
+      <c r="R119">
+        <v>50</v>
+      </c>
+      <c r="S119">
+        <v>2400</v>
+      </c>
       <c r="V119" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="120" spans="1:22">
+      <c r="W119">
+        <v>1</v>
+      </c>
+      <c r="X119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:24">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -8098,11 +8350,23 @@
       <c r="Q120">
         <v>8.199999999999999</v>
       </c>
+      <c r="R120">
+        <v>0</v>
+      </c>
+      <c r="S120">
+        <v>1700</v>
+      </c>
       <c r="V120" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="121" spans="1:22">
+      <c r="W120">
+        <v>1</v>
+      </c>
+      <c r="X120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -8151,11 +8415,23 @@
       <c r="Q121">
         <v>6.8</v>
       </c>
+      <c r="R121">
+        <v>0</v>
+      </c>
+      <c r="S121">
+        <v>1800</v>
+      </c>
       <c r="V121" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="122" spans="1:22">
+      <c r="W121">
+        <v>1</v>
+      </c>
+      <c r="X121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -8204,11 +8480,23 @@
       <c r="Q122">
         <v>6.8</v>
       </c>
+      <c r="R122">
+        <v>0</v>
+      </c>
+      <c r="S122">
+        <v>1900</v>
+      </c>
       <c r="V122" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="123" spans="1:22">
+      <c r="W122">
+        <v>1</v>
+      </c>
+      <c r="X122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -8257,11 +8545,23 @@
       <c r="Q123">
         <v>8.9</v>
       </c>
+      <c r="R123">
+        <v>0</v>
+      </c>
+      <c r="S123">
+        <v>2100</v>
+      </c>
       <c r="V123" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="124" spans="1:22">
+      <c r="W123">
+        <v>1</v>
+      </c>
+      <c r="X123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -8310,11 +8610,23 @@
       <c r="Q124">
         <v>8.9</v>
       </c>
+      <c r="R124">
+        <v>0</v>
+      </c>
+      <c r="S124">
+        <v>2200</v>
+      </c>
       <c r="V124" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="125" spans="1:22">
+      <c r="W124">
+        <v>1</v>
+      </c>
+      <c r="X124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -8363,8 +8675,20 @@
       <c r="Q125">
         <v>8.1</v>
       </c>
+      <c r="R125">
+        <v>0</v>
+      </c>
+      <c r="S125">
+        <v>2300</v>
+      </c>
       <c r="V125" t="s">
         <v>276</v>
+      </c>
+      <c r="W125">
+        <v>1</v>
+      </c>
+      <c r="X125">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update work november 4th with wide scan
</commit_message>
<xml_diff>
--- a/notebookscc/ana_summer2021/logbooks/auxtelholologbook_2021_07_07_v4.0.xlsx
+++ b/notebookscc/ana_summer2021/logbooks/auxtelholologbook_2021_07_07_v4.0.xlsx
@@ -1397,7 +1397,7 @@
         <v>600</v>
       </c>
       <c r="S3">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="V3" t="s">
         <v>276</v>
@@ -3182,11 +3182,23 @@
       <c r="Q32">
         <v>4.5</v>
       </c>
+      <c r="R32">
+        <v>2700</v>
+      </c>
+      <c r="S32">
+        <v>3400</v>
+      </c>
       <c r="V32" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="33" spans="1:22">
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3235,11 +3247,23 @@
       <c r="Q33">
         <v>5.3</v>
       </c>
+      <c r="R33">
+        <v>2100</v>
+      </c>
+      <c r="S33">
+        <v>200</v>
+      </c>
       <c r="V33" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="34" spans="1:22">
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3288,11 +3312,23 @@
       <c r="Q34">
         <v>5.3</v>
       </c>
+      <c r="R34">
+        <v>2100</v>
+      </c>
+      <c r="S34">
+        <v>800</v>
+      </c>
       <c r="V34" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="35" spans="1:22">
+      <c r="W34">
+        <v>1</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3341,11 +3377,23 @@
       <c r="Q35">
         <v>4.4</v>
       </c>
+      <c r="R35">
+        <v>2100</v>
+      </c>
+      <c r="S35">
+        <v>1400</v>
+      </c>
       <c r="V35" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="36" spans="1:22">
+      <c r="W35">
+        <v>1</v>
+      </c>
+      <c r="X35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3394,11 +3442,23 @@
       <c r="Q36">
         <v>5.1</v>
       </c>
+      <c r="R36">
+        <v>2200</v>
+      </c>
+      <c r="S36">
+        <v>2000</v>
+      </c>
       <c r="V36" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="37" spans="1:22">
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3447,11 +3507,23 @@
       <c r="Q37">
         <v>5.1</v>
       </c>
+      <c r="R37">
+        <v>2200</v>
+      </c>
+      <c r="S37">
+        <v>2700</v>
+      </c>
       <c r="V37" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="38" spans="1:22">
+      <c r="W37">
+        <v>1</v>
+      </c>
+      <c r="X37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3500,11 +3572,23 @@
       <c r="Q38">
         <v>4.8</v>
       </c>
+      <c r="R38">
+        <v>2200</v>
+      </c>
+      <c r="S38">
+        <v>3300</v>
+      </c>
       <c r="V38" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="39" spans="1:22">
+      <c r="W38">
+        <v>1</v>
+      </c>
+      <c r="X38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3553,11 +3637,23 @@
       <c r="Q39">
         <v>4.8</v>
       </c>
+      <c r="R39">
+        <v>1500</v>
+      </c>
+      <c r="S39">
+        <v>100</v>
+      </c>
       <c r="V39" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="40" spans="1:22">
+      <c r="W39">
+        <v>1</v>
+      </c>
+      <c r="X39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3606,11 +3702,23 @@
       <c r="Q40">
         <v>4.6</v>
       </c>
+      <c r="R40">
+        <v>1500</v>
+      </c>
+      <c r="S40">
+        <v>700</v>
+      </c>
       <c r="V40" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="41" spans="1:22">
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="X40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3659,11 +3767,23 @@
       <c r="Q41">
         <v>4.1</v>
       </c>
+      <c r="R41">
+        <v>1500</v>
+      </c>
+      <c r="S41">
+        <v>1300</v>
+      </c>
       <c r="V41" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="42" spans="1:22">
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="X41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3712,11 +3832,23 @@
       <c r="Q42">
         <v>4.1</v>
       </c>
+      <c r="R42">
+        <v>1500</v>
+      </c>
+      <c r="S42">
+        <v>1900</v>
+      </c>
       <c r="V42" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="43" spans="1:22">
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3765,11 +3897,23 @@
       <c r="Q43">
         <v>4</v>
       </c>
+      <c r="R43">
+        <v>1500</v>
+      </c>
+      <c r="S43">
+        <v>2500</v>
+      </c>
       <c r="V43" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="44" spans="1:22">
+      <c r="W43">
+        <v>1</v>
+      </c>
+      <c r="X43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3818,11 +3962,23 @@
       <c r="Q44">
         <v>4.2</v>
       </c>
+      <c r="R44">
+        <v>1500</v>
+      </c>
+      <c r="S44">
+        <v>3100</v>
+      </c>
       <c r="V44" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="45" spans="1:22">
+      <c r="W44">
+        <v>1</v>
+      </c>
+      <c r="X44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3875,7 +4031,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:24">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3924,11 +4080,23 @@
       <c r="Q46">
         <v>5.3</v>
       </c>
+      <c r="R46">
+        <v>800</v>
+      </c>
+      <c r="S46">
+        <v>600</v>
+      </c>
       <c r="V46" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="47" spans="1:22">
+      <c r="W46">
+        <v>1</v>
+      </c>
+      <c r="X46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3977,11 +4145,23 @@
       <c r="Q47">
         <v>4.8</v>
       </c>
+      <c r="R47">
+        <v>800</v>
+      </c>
+      <c r="S47">
+        <v>1200</v>
+      </c>
       <c r="V47" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="48" spans="1:22">
+      <c r="W47">
+        <v>1</v>
+      </c>
+      <c r="X47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4030,11 +4210,23 @@
       <c r="Q48">
         <v>4.8</v>
       </c>
+      <c r="R48">
+        <v>800</v>
+      </c>
+      <c r="S48">
+        <v>1800</v>
+      </c>
       <c r="V48" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="49" spans="1:22">
+      <c r="W48">
+        <v>1</v>
+      </c>
+      <c r="X48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4083,11 +4275,23 @@
       <c r="Q49">
         <v>3.6</v>
       </c>
+      <c r="R49">
+        <v>800</v>
+      </c>
+      <c r="S49">
+        <v>2400</v>
+      </c>
       <c r="V49" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="50" spans="1:22">
+      <c r="W49">
+        <v>1</v>
+      </c>
+      <c r="X49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4136,11 +4340,23 @@
       <c r="Q50">
         <v>3.6</v>
       </c>
+      <c r="R50">
+        <v>800</v>
+      </c>
+      <c r="S50">
+        <v>3000</v>
+      </c>
       <c r="V50" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="51" spans="1:22">
+      <c r="W50">
+        <v>1</v>
+      </c>
+      <c r="X50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4193,7 +4409,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:22">
+    <row r="52" spans="1:24">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4242,11 +4458,23 @@
       <c r="Q52">
         <v>5.5</v>
       </c>
+      <c r="R52">
+        <v>300</v>
+      </c>
+      <c r="S52">
+        <v>500</v>
+      </c>
       <c r="V52" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="53" spans="1:22">
+      <c r="W52">
+        <v>1</v>
+      </c>
+      <c r="X52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4295,11 +4523,23 @@
       <c r="Q53">
         <v>5.5</v>
       </c>
+      <c r="R53">
+        <v>300</v>
+      </c>
+      <c r="S53">
+        <v>1100</v>
+      </c>
       <c r="V53" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="54" spans="1:22">
+      <c r="W53">
+        <v>1</v>
+      </c>
+      <c r="X53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4348,11 +4588,23 @@
       <c r="Q54">
         <v>3.8</v>
       </c>
+      <c r="R54">
+        <v>200</v>
+      </c>
+      <c r="S54">
+        <v>1700</v>
+      </c>
       <c r="V54" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="55" spans="1:22">
+      <c r="W54">
+        <v>1</v>
+      </c>
+      <c r="X54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4401,11 +4653,23 @@
       <c r="Q55">
         <v>3.8</v>
       </c>
+      <c r="R55">
+        <v>300</v>
+      </c>
+      <c r="S55">
+        <v>2300</v>
+      </c>
       <c r="V55" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="56" spans="1:22">
+      <c r="W55">
+        <v>1</v>
+      </c>
+      <c r="X55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4454,11 +4718,23 @@
       <c r="Q56">
         <v>3.8</v>
       </c>
+      <c r="R56">
+        <v>200</v>
+      </c>
+      <c r="S56">
+        <v>2900</v>
+      </c>
       <c r="V56" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="57" spans="1:22">
+      <c r="W56">
+        <v>1</v>
+      </c>
+      <c r="X56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4507,11 +4783,23 @@
       <c r="Q57">
         <v>5.7</v>
       </c>
+      <c r="R57">
+        <v>200</v>
+      </c>
+      <c r="S57">
+        <v>3500</v>
+      </c>
       <c r="V57" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="58" spans="1:22">
+      <c r="W57">
+        <v>1</v>
+      </c>
+      <c r="X57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4560,11 +4848,23 @@
       <c r="Q58">
         <v>2.5</v>
       </c>
+      <c r="R58">
+        <v>300</v>
+      </c>
+      <c r="S58">
+        <v>2200</v>
+      </c>
       <c r="V58" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="59" spans="1:22">
+      <c r="W58">
+        <v>1</v>
+      </c>
+      <c r="X58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4613,11 +4913,23 @@
       <c r="Q59">
         <v>4.8</v>
       </c>
+      <c r="R59">
+        <v>300</v>
+      </c>
+      <c r="S59">
+        <v>2300</v>
+      </c>
       <c r="V59" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="60" spans="1:22">
+      <c r="W59">
+        <v>1</v>
+      </c>
+      <c r="X59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4670,7 +4982,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="1:22">
+    <row r="61" spans="1:24">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4723,7 +5035,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="62" spans="1:22">
+    <row r="62" spans="1:24">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4772,11 +5084,23 @@
       <c r="Q62">
         <v>4.7</v>
       </c>
+      <c r="R62">
+        <v>700</v>
+      </c>
+      <c r="S62">
+        <v>100</v>
+      </c>
       <c r="V62" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="63" spans="1:22">
+      <c r="W62">
+        <v>1</v>
+      </c>
+      <c r="X62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4825,11 +5149,23 @@
       <c r="Q63">
         <v>5.2</v>
       </c>
+      <c r="R63">
+        <v>700</v>
+      </c>
+      <c r="S63">
+        <v>200</v>
+      </c>
       <c r="V63" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="64" spans="1:22">
+      <c r="W63">
+        <v>1</v>
+      </c>
+      <c r="X63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4878,8 +5214,20 @@
       <c r="Q64">
         <v>5.2</v>
       </c>
+      <c r="R64">
+        <v>700</v>
+      </c>
+      <c r="S64">
+        <v>300</v>
+      </c>
       <c r="V64" t="s">
         <v>276</v>
+      </c>
+      <c r="W64">
+        <v>1</v>
+      </c>
+      <c r="X64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:24">
@@ -4931,8 +5279,20 @@
       <c r="Q65">
         <v>4.3</v>
       </c>
+      <c r="R65">
+        <v>700</v>
+      </c>
+      <c r="S65">
+        <v>400</v>
+      </c>
       <c r="V65" t="s">
         <v>276</v>
+      </c>
+      <c r="W65">
+        <v>1</v>
+      </c>
+      <c r="X65">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:24">
@@ -4984,8 +5344,20 @@
       <c r="Q66">
         <v>4.3</v>
       </c>
+      <c r="R66">
+        <v>700</v>
+      </c>
+      <c r="S66">
+        <v>500</v>
+      </c>
       <c r="V66" t="s">
         <v>276</v>
+      </c>
+      <c r="W66">
+        <v>1</v>
+      </c>
+      <c r="X66">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:24">
@@ -5196,8 +5568,20 @@
       <c r="Q70">
         <v>3.9</v>
       </c>
+      <c r="R70">
+        <v>600</v>
+      </c>
+      <c r="S70">
+        <v>100</v>
+      </c>
       <c r="V70" t="s">
         <v>276</v>
+      </c>
+      <c r="W70">
+        <v>1</v>
+      </c>
+      <c r="X70">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:24">
@@ -5249,8 +5633,20 @@
       <c r="Q71">
         <v>4.1</v>
       </c>
+      <c r="R71">
+        <v>600</v>
+      </c>
+      <c r="S71">
+        <v>200</v>
+      </c>
       <c r="V71" t="s">
         <v>276</v>
+      </c>
+      <c r="W71">
+        <v>1</v>
+      </c>
+      <c r="X71">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:24">
@@ -5302,8 +5698,20 @@
       <c r="Q72">
         <v>4.3</v>
       </c>
+      <c r="R72">
+        <v>650</v>
+      </c>
+      <c r="S72">
+        <v>250</v>
+      </c>
       <c r="V72" t="s">
         <v>276</v>
+      </c>
+      <c r="W72">
+        <v>1</v>
+      </c>
+      <c r="X72">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:24">
@@ -5355,8 +5763,20 @@
       <c r="Q73">
         <v>4.3</v>
       </c>
+      <c r="R73">
+        <v>650</v>
+      </c>
+      <c r="S73">
+        <v>350</v>
+      </c>
       <c r="V73" t="s">
         <v>276</v>
+      </c>
+      <c r="W73">
+        <v>1</v>
+      </c>
+      <c r="X73">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:24">
@@ -5408,8 +5828,20 @@
       <c r="Q74">
         <v>5</v>
       </c>
+      <c r="R74">
+        <v>1300</v>
+      </c>
+      <c r="S74">
+        <v>3400</v>
+      </c>
       <c r="V74" t="s">
         <v>276</v>
+      </c>
+      <c r="W74">
+        <v>1</v>
+      </c>
+      <c r="X74">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:24">

</xml_diff>